<commit_message>
Add word choose in main & Add var_frame
</commit_message>
<xml_diff>
--- a/the_word.xlsx
+++ b/the_word.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linyuxiang/Desktop/code/Learning_Japanese/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E3FAE7-ECAB-A343-90EE-4FBFF69199DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96B5049-635F-FF46-BC4F-D01E0D452D1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{60B39602-CA03-F040-8524-C5DD9C0222AC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2625" uniqueCount="1874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2626" uniqueCount="1874">
   <si>
     <t>あし</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7626,8 +7626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D03D34A-BA0A-4C4B-8E51-02C16EDC5D6C}">
   <dimension ref="A1:BV82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="183" zoomScaleNormal="222" workbookViewId="0">
-      <selection activeCell="BM2" sqref="BM2"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="183" zoomScaleNormal="222" workbookViewId="0">
+      <selection activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7708,6 +7708,9 @@
       </c>
       <c r="Z1" t="s">
         <v>1872</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>1873</v>
       </c>
       <c r="AB1" t="s">
         <v>734</v>

</xml_diff>